<commit_message>
Main page window full screen
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC2E8A3-07B2-E149-A93F-54C13DE37E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75344AA9-4993-4D43-8CF9-3C461467A011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="422">
   <si>
     <t>DIN</t>
   </si>
@@ -1253,6 +1253,39 @@
   </si>
   <si>
     <t>771313000253</t>
+  </si>
+  <si>
+    <t>068510020406</t>
+  </si>
+  <si>
+    <t>068510021403</t>
+  </si>
+  <si>
+    <t>055873030258</t>
+  </si>
+  <si>
+    <t>055873030500</t>
+  </si>
+  <si>
+    <t>068510345400</t>
+  </si>
+  <si>
+    <t>060025418891</t>
+  </si>
+  <si>
+    <t>057606111340</t>
+  </si>
+  <si>
+    <t>057606111357</t>
+  </si>
+  <si>
+    <t>068510899279</t>
+  </si>
+  <si>
+    <t>771313157285</t>
+  </si>
+  <si>
+    <t>057606781840</t>
   </si>
 </sst>
 </file>
@@ -1667,7 +1700,7 @@
   <dimension ref="A1:F200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1813,6 +1846,9 @@
       <c r="D9" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="E9" s="7" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -1827,6 +1863,9 @@
       <c r="D10" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="E10" s="7" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1886,6 +1925,9 @@
       <c r="D14" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="E14" s="7" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -2347,6 +2389,9 @@
       <c r="D46" s="2" t="s">
         <v>385</v>
       </c>
+      <c r="E46" s="7" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
@@ -3373,6 +3418,9 @@
       <c r="D117" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="E117" s="7" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
@@ -3387,6 +3435,9 @@
       <c r="D118" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="E118" s="7" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
@@ -3445,7 +3496,9 @@
       <c r="D122" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E122" s="9"/>
+      <c r="E122" s="9" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
@@ -4016,7 +4069,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>318</v>
       </c>
@@ -4030,7 +4083,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>320</v>
       </c>
@@ -4044,7 +4097,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>322</v>
       </c>
@@ -4058,7 +4111,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>322</v>
       </c>
@@ -4072,7 +4125,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>325</v>
       </c>
@@ -4086,7 +4139,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>327</v>
       </c>
@@ -4100,7 +4153,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>329</v>
       </c>
@@ -4114,7 +4167,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>331</v>
       </c>
@@ -4127,8 +4180,11 @@
       <c r="D168" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E168" s="7" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>331</v>
       </c>
@@ -4141,8 +4197,11 @@
       <c r="D169" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E169" s="7" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>334</v>
       </c>
@@ -4155,8 +4214,11 @@
       <c r="D170" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E170" s="7" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>334</v>
       </c>
@@ -4170,7 +4232,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>337</v>
       </c>
@@ -4183,8 +4245,11 @@
       <c r="D172" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E172" s="7" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>339</v>
       </c>
@@ -4198,7 +4263,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>339</v>
       </c>
@@ -4212,7 +4277,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>342</v>
       </c>
@@ -4226,7 +4291,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>342</v>
       </c>
@@ -4595,5 +4660,8 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="E117" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more upc and new meds, also cleaned my dicionnary of spaces in front of data
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E9ED788-9E96-E44C-BA07-2EE7C2866B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6ADEBFB-0D38-4E4F-96AC-0BDF646E5308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="493">
   <si>
     <t>DIN</t>
   </si>
@@ -1458,13 +1458,67 @@
   </si>
   <si>
     <t>660933002320</t>
+  </si>
+  <si>
+    <t>055860010157</t>
+  </si>
+  <si>
+    <t>064589001926</t>
+  </si>
+  <si>
+    <t>064589002138</t>
+  </si>
+  <si>
+    <t>064589000752</t>
+  </si>
+  <si>
+    <t>064589001643</t>
+  </si>
+  <si>
+    <t>771313005487</t>
+  </si>
+  <si>
+    <t>771313258241</t>
+  </si>
+  <si>
+    <t>771313005524</t>
+  </si>
+  <si>
+    <t>057606818720</t>
+  </si>
+  <si>
+    <t>057606819529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	00728209</t>
+  </si>
+  <si>
+    <t>057606820921</t>
+  </si>
+  <si>
+    <t>MOGADON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	00511528</t>
+  </si>
+  <si>
+    <t>660933001712</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	02533669</t>
+  </si>
+  <si>
+    <t>771313253949</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	APO-METHADONE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1492,13 +1546,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1508,7 +1555,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1551,24 +1598,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1583,10 +1617,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1892,10 +1922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F207"/>
+  <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A191" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2166,7 +2196,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -2180,7 +2210,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>44</v>
       </c>
@@ -2193,8 +2223,14 @@
       <c r="D18" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="F18" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -2207,8 +2243,14 @@
       <c r="D19" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="F19" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>44</v>
       </c>
@@ -2222,169 +2264,175 @@
         <v>380</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D24" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D27" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="D31" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>380</v>
@@ -2392,13 +2440,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>380</v>
@@ -2409,10 +2457,10 @@
         <v>74</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>380</v>
@@ -2420,13 +2468,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>380</v>
@@ -2434,27 +2482,27 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>384</v>
@@ -2462,27 +2510,27 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>380</v>
@@ -2490,19 +2538,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>403</v>
+        <v>380</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2510,16 +2555,16 @@
         <v>89</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2527,16 +2572,16 @@
         <v>89</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2544,16 +2589,16 @@
         <v>89</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
@@ -2561,13 +2606,16 @@
         <v>89</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>383</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2575,10 +2623,10 @@
         <v>89</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>383</v>
@@ -2589,61 +2637,61 @@
         <v>89</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>407</v>
+        <v>96</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>383</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>99</v>
+        <v>408</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>407</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>416</v>
-      </c>
-      <c r="F47" s="2">
-        <v>4</v>
+        <v>409</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>385</v>
       </c>
+      <c r="E48" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="F48" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>385</v>
@@ -2651,28 +2699,28 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>384</v>
@@ -2681,16 +2729,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E52" s="7"/>
     </row>
@@ -2699,10 +2747,10 @@
         <v>114</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>383</v>
@@ -2711,13 +2759,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>117</v>
+        <v>29</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>383</v>
@@ -2726,13 +2774,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>383</v>
@@ -2744,10 +2792,10 @@
         <v>121</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>383</v>
@@ -2759,10 +2807,10 @@
         <v>121</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>124</v>
+        <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>383</v>
@@ -2771,39 +2819,34 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>434</v>
-      </c>
-      <c r="F58" s="2">
-        <v>100</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>126</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F59" s="2">
         <v>100</v>
@@ -2814,16 +2857,16 @@
         <v>126</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F60" s="2">
         <v>100</v>
@@ -2834,16 +2877,16 @@
         <v>126</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F61" s="2">
         <v>100</v>
@@ -2851,100 +2894,105 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E62" s="7"/>
+        <v>380</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F62" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>430</v>
+        <v>132</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>137</v>
+        <v>430</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>142</v>
+        <v>68</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>60</v>
@@ -2952,19 +3000,14 @@
       <c r="D68" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="F68" s="2">
-        <v>100</v>
-      </c>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>60</v>
@@ -2973,7 +3016,7 @@
         <v>380</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F69" s="2">
         <v>100</v>
@@ -2984,16 +3027,16 @@
         <v>149</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F70" s="2">
         <v>100</v>
@@ -3004,16 +3047,16 @@
         <v>149</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F71" s="2">
         <v>100</v>
@@ -3021,19 +3064,19 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="F72" s="2">
         <v>100</v>
@@ -3044,16 +3087,16 @@
         <v>153</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>155</v>
+        <v>39</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F73" s="2">
         <v>100</v>
@@ -3064,16 +3107,16 @@
         <v>153</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F74" s="2">
         <v>100</v>
@@ -3084,40 +3127,45 @@
         <v>153</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>158</v>
+        <v>46</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E75" s="7"/>
+      <c r="E75" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="F75" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>384</v>
@@ -3126,28 +3174,28 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>383</v>
@@ -3156,13 +3204,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>383</v>
@@ -3171,42 +3219,37 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>58</v>
+        <v>172</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E81" s="7" t="s">
-        <v>442</v>
-      </c>
-      <c r="F81" s="2">
-        <v>100</v>
-      </c>
+      <c r="E81" s="7"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E82" s="11" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="F82" s="2">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -3214,16 +3257,16 @@
         <v>178</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>453</v>
+        <v>176</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>455</v>
+        <v>177</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F83" s="2">
         <v>60</v>
@@ -3234,16 +3277,16 @@
         <v>178</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F84" s="2">
         <v>60</v>
@@ -3254,16 +3297,16 @@
         <v>178</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E85" s="6" t="s">
-        <v>452</v>
+      <c r="E85" s="11" t="s">
+        <v>451</v>
       </c>
       <c r="F85" s="2">
         <v>60</v>
@@ -3271,36 +3314,36 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>179</v>
+        <v>458</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>163</v>
+        <v>454</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>452</v>
+      </c>
+      <c r="F86" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>31</v>
+        <v>163</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="F87" s="2">
-        <v>60</v>
+        <v>384</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -3308,16 +3351,16 @@
         <v>182</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>184</v>
+        <v>31</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F88" s="2">
         <v>60</v>
@@ -3328,16 +3371,16 @@
         <v>182</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>41</v>
+        <v>184</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F89" s="2">
         <v>60</v>
@@ -3348,16 +3391,16 @@
         <v>182</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>187</v>
+        <v>41</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="F90" s="2">
         <v>60</v>
@@ -3368,16 +3411,16 @@
         <v>182</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>56</v>
+        <v>187</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="F91" s="2">
         <v>60</v>
@@ -3388,16 +3431,16 @@
         <v>182</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>190</v>
+        <v>56</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="F92" s="2">
         <v>60</v>
@@ -3405,27 +3448,33 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>71</v>
+        <v>190</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="F93" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>380</v>
@@ -3433,22 +3482,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>432</v>
-      </c>
-      <c r="F95" s="2">
-        <v>100</v>
+        <v>380</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -3456,16 +3499,16 @@
         <v>196</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F96" s="2">
         <v>100</v>
@@ -3476,19 +3519,19 @@
         <v>196</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="F97" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -3496,24 +3539,30 @@
         <v>196</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>34</v>
+        <v>199</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>383</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>431</v>
+      </c>
+      <c r="F98" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>117</v>
+        <v>34</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>383</v>
@@ -3521,13 +3570,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>204</v>
+        <v>117</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>383</v>
@@ -3535,22 +3584,22 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>29</v>
+        <v>204</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F101" s="2">
-        <v>100</v>
+        <v>250</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -3558,16 +3607,16 @@
         <v>207</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F102" s="2">
         <v>100</v>
@@ -3575,30 +3624,36 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>380</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F103" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
@@ -3606,10 +3661,10 @@
         <v>212</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>383</v>
@@ -3620,10 +3675,10 @@
         <v>212</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>383</v>
@@ -3634,10 +3689,10 @@
         <v>212</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>199</v>
+        <v>95</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>383</v>
@@ -3648,10 +3703,10 @@
         <v>212</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>58</v>
+        <v>199</v>
       </c>
       <c r="D108" s="2" t="s">
         <v>383</v>
@@ -3659,27 +3714,27 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>380</v>
@@ -3690,10 +3745,10 @@
         <v>220</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>380</v>
@@ -3701,24 +3756,24 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>223</v>
+        <v>34</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>223</v>
@@ -3729,55 +3784,55 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>26</v>
+        <v>223</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>230</v>
+        <v>26</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>68</v>
+        <v>230</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>380</v>
@@ -3788,10 +3843,10 @@
         <v>235</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="D118" s="2" t="s">
         <v>380</v>
@@ -3802,10 +3857,10 @@
         <v>235</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>4</v>
+        <v>93</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>380</v>
@@ -3813,36 +3868,30 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="C120" s="2" t="s">
+      <c r="C121" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D120" s="2" t="s">
+      <c r="D121" s="2" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C121" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E121" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="F121" s="2">
-        <v>30</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -3850,33 +3899,39 @@
         <v>241</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F122" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="2" t="s">
-        <v>244</v>
+      <c r="A123" s="8" t="s">
+        <v>241</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>380</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="F123" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
@@ -3884,16 +3939,13 @@
         <v>244</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -3901,36 +3953,33 @@
         <v>244</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="F126" s="2">
-        <v>500</v>
+        <v>424</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -3947,27 +3996,27 @@
         <v>380</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="F127" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>155</v>
+        <v>29</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>462</v>
+        <v>428</v>
       </c>
       <c r="F128" s="2">
         <v>100</v>
@@ -3978,16 +4027,16 @@
         <v>250</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>39</v>
+        <v>155</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E129" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F129" s="2">
         <v>100</v>
@@ -3998,16 +4047,16 @@
         <v>250</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F130" s="2">
         <v>100</v>
@@ -4018,16 +4067,16 @@
         <v>250</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>466</v>
+        <v>252</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>158</v>
+        <v>46</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>380</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F131" s="2">
         <v>100</v>
@@ -4035,30 +4084,36 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>253</v>
+        <v>466</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>384</v>
+        <v>380</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>465</v>
+      </c>
+      <c r="F132" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>29</v>
+        <v>163</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -4066,55 +4121,73 @@
         <v>256</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>380</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="F134" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>380</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="F135" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>260</v>
+        <v>485</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="F136" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -4122,10 +4195,10 @@
         <v>261</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>383</v>
@@ -4133,41 +4206,41 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>380</v>
@@ -4175,13 +4248,13 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>270</v>
+        <v>60</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>380</v>
@@ -4189,92 +4262,101 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>273</v>
+        <v>34</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="E143" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="F143" s="2">
-        <v>500</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E145" s="7"/>
+        <v>380</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="F145" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>169</v>
+        <v>276</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E146" s="7"/>
+      <c r="E146" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="F146" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>172</v>
+        <v>276</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E147" s="7"/>
+      <c r="E147" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="F147" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>58</v>
+        <v>166</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>383</v>
@@ -4283,13 +4365,13 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>383</v>
@@ -4298,70 +4380,64 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>34</v>
+        <v>172</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E150" s="11" t="s">
-        <v>390</v>
-      </c>
+      <c r="E150" s="11"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E151" s="11" t="s">
-        <v>391</v>
-      </c>
+      <c r="E151" s="11"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>56</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E152" s="11" t="s">
-        <v>389</v>
-      </c>
+        <v>383</v>
+      </c>
+      <c r="E152" s="11"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>288</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>392</v>
+        <v>287</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>393</v>
+        <v>34</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="E153" s="6" t="s">
-        <v>394</v>
+      <c r="E153" s="11" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -4369,13 +4445,16 @@
         <v>288</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>177</v>
+        <v>4</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>383</v>
+      </c>
+      <c r="E154" s="11" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
@@ -4383,16 +4462,16 @@
         <v>288</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>398</v>
+        <v>290</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E155" s="6" t="s">
-        <v>399</v>
+        <v>380</v>
+      </c>
+      <c r="E155" s="11" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -4400,142 +4479,148 @@
         <v>288</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E156" s="6" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>293</v>
+        <v>177</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E157" s="6" t="s">
-        <v>447</v>
-      </c>
-      <c r="F157" s="2">
-        <v>5</v>
+        <v>383</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>296</v>
+        <v>397</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>398</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
+      </c>
+      <c r="E158" s="6" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>298</v>
+        <v>400</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>299</v>
+        <v>401</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
+      </c>
+      <c r="E159" s="6" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E160" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="F160" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D161" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="B160" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="C160" s="2" t="s">
+      <c r="C163" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D160" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="2" t="s">
+      <c r="D163" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="B161" s="4" t="s">
+      <c r="B164" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="C161" s="2" t="s">
+      <c r="C164" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D161" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="2" t="s">
+      <c r="D164" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B165" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B165" s="4" t="s">
-        <v>310</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>34</v>
@@ -4544,12 +4629,12 @@
         <v>380</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>60</v>
@@ -4558,241 +4643,229 @@
         <v>380</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D167" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B167" s="4" t="s">
+      <c r="B170" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C170" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D167" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
+      <c r="D170" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="B168" s="4" t="s">
+      <c r="B171" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="C168" s="2" t="s">
+      <c r="C171" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D168" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
+      <c r="D171" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="B169" s="4" t="s">
+      <c r="B172" s="4" t="s">
         <v>316</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C172" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D169" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
+      <c r="D172" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="B170" s="4" t="s">
+      <c r="B173" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="C170" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D170" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
+      <c r="D173" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B171" s="4" t="s">
+      <c r="B174" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C174" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D171" s="2" t="s">
+      <c r="D174" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B172" s="4" t="s">
+      <c r="B175" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C175" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D172" s="2" t="s">
+      <c r="D175" s="2" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B173" s="4" t="s">
+      <c r="B176" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D173" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="2" t="s">
+      <c r="D176" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B174" s="4" t="s">
+      <c r="B177" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="C174" s="2" t="s">
+      <c r="C177" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D174" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A175" s="2" t="s">
+      <c r="D177" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B175" s="4" t="s">
+      <c r="B178" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C178" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D175" s="2" t="s">
+      <c r="D178" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A176" s="8" t="s">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="B176" s="4" t="s">
+      <c r="B179" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="C176" s="2" t="s">
+      <c r="C179" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D176" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E176" s="6" t="s">
+      <c r="D179" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E179" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="F176" s="2">
+      <c r="F179" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="8" t="s">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="B177" s="4" t="s">
+      <c r="B180" s="4" t="s">
         <v>332</v>
       </c>
-      <c r="C177" s="2" t="s">
+      <c r="C180" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D177" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E177" s="6" t="s">
+      <c r="D180" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E180" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="F177" s="2">
+      <c r="F180" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A178" s="8" t="s">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="B178" s="4" t="s">
+      <c r="B181" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="C178" s="2" t="s">
+      <c r="C181" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D178" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E178" s="6" t="s">
+      <c r="D181" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E181" s="6" t="s">
         <v>415</v>
-      </c>
-      <c r="F178" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A179" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="B179" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A180" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="B180" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="C180" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E180" s="6" t="s">
-        <v>419</v>
-      </c>
-      <c r="F180" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A181" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C181" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E181" s="6" t="s">
-        <v>422</v>
       </c>
       <c r="F181" s="2">
         <v>100</v>
@@ -4800,391 +4873,494 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B182" s="4" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="E182" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="F182" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>293</v>
+        <v>34</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="E183" s="6" t="s">
-        <v>448</v>
+        <v>419</v>
       </c>
       <c r="F183" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>296</v>
+        <v>58</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>385</v>
+        <v>380</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="F184" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>345</v>
+        <v>56</v>
       </c>
       <c r="D185" s="2" t="s">
         <v>380</v>
+      </c>
+      <c r="E185" s="6" t="s">
+        <v>423</v>
+      </c>
+      <c r="F185" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>348</v>
+        <v>293</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>380</v>
+        <v>385</v>
+      </c>
+      <c r="E186" s="6" t="s">
+        <v>448</v>
+      </c>
+      <c r="F186" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>46</v>
+        <v>296</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="E187" s="7"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>39</v>
+        <v>345</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E188" s="11"/>
+      <c r="E188" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="F188" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>29</v>
+        <v>348</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="E189" s="11"/>
+      <c r="E189" s="11" t="s">
+        <v>479</v>
+      </c>
+      <c r="F189" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="E190" s="11"/>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="E191" s="11"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D192" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E192" s="11"/>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D193" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D194" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B193" s="4" t="s">
+      <c r="B195" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D195" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E195" s="11"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B196" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="C193" s="2" t="s">
+      <c r="C196" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D193" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A194" s="2" t="s">
+      <c r="D196" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="B194" s="4" t="s">
+      <c r="B197" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C194" s="2" t="s">
+      <c r="C197" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D194" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
+      <c r="D197" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B195" s="4" t="s">
+      <c r="B198" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="C195" s="2" t="s">
+      <c r="C198" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D195" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
+      <c r="D198" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E198" s="7"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B196" s="4" t="s">
+      <c r="B199" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C196" s="2" t="s">
+      <c r="C199" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D196" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A197" s="2" t="s">
+      <c r="D199" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E199" s="11"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="B197" s="4" t="s">
+      <c r="B200" s="4" t="s">
         <v>365</v>
       </c>
-      <c r="C197" s="2" t="s">
+      <c r="C200" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="D197" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A198" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B198" s="16" t="s">
-        <v>367</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E198" s="7"/>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A199" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B199" s="4" t="s">
-        <v>369</v>
-      </c>
-      <c r="C199" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E199" s="11"/>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A200" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B200" s="4" t="s">
-        <v>370</v>
-      </c>
-      <c r="C200" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="D200" s="2" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E200" s="11"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B201" s="4" t="s">
-        <v>371</v>
+      <c r="B201" s="12" t="s">
+        <v>367</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E201" s="11"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>368</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>383</v>
       </c>
       <c r="E202" s="7"/>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
         <v>368</v>
       </c>
       <c r="B203" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E203" s="7"/>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D204" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E204" s="11"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D205" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E205" s="11"/>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B206" s="4" t="s">
         <v>373</v>
       </c>
-      <c r="C203" s="2" t="s">
+      <c r="C206" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D203" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E203" s="7"/>
-    </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A204" s="2" t="s">
+      <c r="D206" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E206" s="11"/>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B207" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="C204" s="2" t="s">
+      <c r="C207" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D204" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E204" s="11"/>
-    </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A205" s="2" t="s">
+      <c r="D207" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E207" s="11"/>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="B205" s="4" t="s">
+      <c r="B208" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="C205" s="2" t="s">
+      <c r="C208" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D205" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E205" s="11"/>
-    </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A206" s="1" t="s">
+      <c r="D208" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E208" s="11"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="B206" s="3" t="s">
+      <c r="B209" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="C206" s="1">
+      <c r="C209" s="1">
         <v>1</v>
       </c>
-      <c r="D206" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="E206" s="10" t="s">
+      <c r="D209" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="E209" s="10" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A207" s="12"/>
-      <c r="B207" s="13"/>
-      <c r="C207" s="14"/>
-      <c r="D207" s="14"/>
-      <c r="E207" s="15"/>
-      <c r="F207" s="12"/>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E210" s="11" t="s">
+        <v>489</v>
+      </c>
+      <c r="F210" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E211" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="F211" s="2">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F206">
-    <sortCondition ref="A2:A206"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F209">
+    <sortCondition ref="A2:A209"/>
   </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the remaining drug in my sheet, also set all the pck size, added the next step for excel sheet
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551D94D9-ED55-4342-8574-DFDDCF6DD6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B48ED76-B0D8-B248-BCB6-6866460A0B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="210">
   <si>
     <t>Drug Name</t>
   </si>
@@ -635,6 +635,21 @@
   </si>
   <si>
     <t>Act (if no upc use 1)</t>
+  </si>
+  <si>
+    <t>TARO-TESTOSTERONE INJ</t>
+  </si>
+  <si>
+    <t>INJ</t>
+  </si>
+  <si>
+    <t>TEVA-COTRIDIN EXPECTORANT</t>
+  </si>
+  <si>
+    <t>VIAL</t>
+  </si>
+  <si>
+    <t>SDZ-HYDROMORPHONE IM INJ</t>
   </si>
 </sst>
 </file>
@@ -719,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -731,6 +746,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1035,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1297,6 +1316,9 @@
       <c r="E15">
         <v>771313078801</v>
       </c>
+      <c r="F15" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1314,6 +1336,9 @@
       <c r="E16">
         <v>771313078702</v>
       </c>
+      <c r="F16" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1394,13 +1419,19 @@
         <v>34</v>
       </c>
       <c r="B21" s="2">
-        <v>655767</v>
+        <v>655759</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E21">
+        <v>771313005524</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1408,19 +1439,13 @@
         <v>34</v>
       </c>
       <c r="B22" s="2">
-        <v>655759</v>
+        <v>655767</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E22">
-        <v>771313005524</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,13 +1595,19 @@
         <v>43</v>
       </c>
       <c r="B31" s="2">
-        <v>2366746</v>
+        <v>2306530</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E31">
+        <v>771313221757</v>
+      </c>
+      <c r="F31" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1584,10 +1615,10 @@
         <v>43</v>
       </c>
       <c r="B32" s="2">
-        <v>2366754</v>
+        <v>2366746</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
@@ -1598,19 +1629,13 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>2366762</v>
+        <v>2366754</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E33">
-        <v>771313221740</v>
-      </c>
-      <c r="F33" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1618,16 +1643,16 @@
         <v>43</v>
       </c>
       <c r="B34" s="2">
-        <v>2306530</v>
+        <v>2366762</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E34">
-        <v>771313221757</v>
+        <v>771313221740</v>
       </c>
       <c r="F34" s="2">
         <v>100</v>
@@ -1674,6 +1699,12 @@
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E37">
+        <v>771313256360</v>
+      </c>
+      <c r="F37" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
@@ -1688,6 +1719,12 @@
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E38">
+        <v>771313237703</v>
+      </c>
+      <c r="F38" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
@@ -1730,6 +1767,12 @@
       <c r="D41" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E41" s="9">
+        <v>68625100253</v>
+      </c>
+      <c r="F41" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
@@ -1744,6 +1787,12 @@
       <c r="D42" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E42" s="9">
+        <v>68625100352</v>
+      </c>
+      <c r="F42" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
@@ -1758,6 +1807,12 @@
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E43">
+        <v>886965005492</v>
+      </c>
+      <c r="F43" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
@@ -1772,6 +1827,12 @@
       <c r="D44" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E44">
+        <v>886965002392</v>
+      </c>
+      <c r="F44" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
@@ -1838,16 +1899,16 @@
         <v>61</v>
       </c>
       <c r="B48" s="2">
-        <v>2277182</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>45</v>
+        <v>2277174</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E48">
-        <v>60025101403</v>
+      <c r="E48" s="11">
+        <v>60025101304</v>
       </c>
       <c r="F48" s="2">
         <v>100</v>
@@ -1858,13 +1919,16 @@
         <v>61</v>
       </c>
       <c r="B49" s="2">
-        <v>2277204</v>
+        <v>2277182</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E49">
+        <v>60025101403</v>
       </c>
       <c r="F49" s="2">
         <v>100</v>
@@ -1875,10 +1939,10 @@
         <v>61</v>
       </c>
       <c r="B50" s="2">
-        <v>2277212</v>
+        <v>2277204</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>33</v>
@@ -1893,17 +1957,15 @@
         <v>61</v>
       </c>
       <c r="B51" s="2">
-        <v>2277174</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>41</v>
+        <v>2277212</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E51" s="7">
-        <v>60025101304</v>
-      </c>
+      <c r="E51" s="7"/>
       <c r="F51" s="2">
         <v>100</v>
       </c>
@@ -1971,7 +2033,12 @@
       <c r="D55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="7"/>
+      <c r="E55" s="7">
+        <v>64589001889</v>
+      </c>
+      <c r="F55" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
@@ -2186,7 +2253,12 @@
       <c r="D68" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E68" s="7"/>
+      <c r="E68" s="7">
+        <v>775848181005</v>
+      </c>
+      <c r="F68" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
@@ -2721,6 +2793,12 @@
       <c r="D98" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E98">
+        <v>622082288376</v>
+      </c>
+      <c r="F98" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
@@ -3005,6 +3083,12 @@
       <c r="D114" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E114">
+        <v>697359005734</v>
+      </c>
+      <c r="F114" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
@@ -3053,6 +3137,12 @@
       <c r="D117" s="2" t="s">
         <v>95</v>
       </c>
+      <c r="E117" s="9">
+        <v>30406000304</v>
+      </c>
+      <c r="F117" s="2">
+        <v>1000</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
@@ -3129,6 +3219,12 @@
       <c r="D122" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E122">
+        <v>628791006294</v>
+      </c>
+      <c r="F122" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
@@ -3143,12 +3239,6 @@
       <c r="D123" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E123">
-        <v>628791006294</v>
-      </c>
-      <c r="F123" s="2">
-        <v>100</v>
-      </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
@@ -3211,6 +3301,12 @@
       <c r="D127" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="E127">
+        <v>625972019869</v>
+      </c>
+      <c r="F127" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
@@ -3282,6 +3378,9 @@
       <c r="E131">
         <v>57606872821</v>
       </c>
+      <c r="F131" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
@@ -3299,6 +3398,9 @@
       <c r="E132">
         <v>57606873620</v>
       </c>
+      <c r="F132" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
@@ -3314,10 +3416,10 @@
         <v>8</v>
       </c>
       <c r="E133">
-        <v>57606781840</v>
+        <v>57606781826</v>
       </c>
       <c r="F133" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
@@ -3334,10 +3436,10 @@
         <v>8</v>
       </c>
       <c r="E134">
-        <v>57606781826</v>
+        <v>57606781840</v>
       </c>
       <c r="F134" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -3365,16 +3467,16 @@
         <v>148</v>
       </c>
       <c r="B136" s="2">
-        <v>885436</v>
+        <v>885428</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E136">
-        <v>57606543646</v>
+        <v>57606542847</v>
       </c>
       <c r="F136" s="2">
         <v>100</v>
@@ -3385,16 +3487,16 @@
         <v>148</v>
       </c>
       <c r="B137" s="2">
-        <v>885444</v>
+        <v>885436</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E137">
-        <v>57606544445</v>
+        <v>57606543646</v>
       </c>
       <c r="F137" s="2">
         <v>100</v>
@@ -3405,16 +3507,16 @@
         <v>148</v>
       </c>
       <c r="B138" s="2">
-        <v>885428</v>
+        <v>885444</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E138">
-        <v>57606542847</v>
+        <v>57606544445</v>
       </c>
       <c r="F138" s="2">
         <v>100</v>
@@ -3521,6 +3623,7 @@
       <c r="D144" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E144" s="11"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
@@ -3590,6 +3693,12 @@
       <c r="D148" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E148" s="9">
+        <v>57606025876</v>
+      </c>
+      <c r="F148" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
@@ -3659,10 +3768,10 @@
         <v>33</v>
       </c>
       <c r="E152">
-        <v>64589001926</v>
+        <v>64589002138</v>
       </c>
       <c r="F152" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
@@ -3679,10 +3788,10 @@
         <v>33</v>
       </c>
       <c r="E153">
-        <v>64589002138</v>
+        <v>64589001926</v>
       </c>
       <c r="F153" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -3698,6 +3807,12 @@
       <c r="D154" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E154" s="9">
+        <v>64589000936</v>
+      </c>
+      <c r="F154" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
@@ -3712,6 +3827,12 @@
       <c r="D155" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E155" s="9">
+        <v>64589002305</v>
+      </c>
+      <c r="F155" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
@@ -3726,6 +3847,12 @@
       <c r="D156" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E156" s="9">
+        <v>64589002299</v>
+      </c>
+      <c r="F156" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
@@ -3772,16 +3899,19 @@
         <v>165</v>
       </c>
       <c r="B159" s="2">
-        <v>2457296</v>
+        <v>2457288</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E159">
-        <v>57513217937</v>
+        <v>57513217920</v>
+      </c>
+      <c r="F159" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -3789,16 +3919,19 @@
         <v>165</v>
       </c>
       <c r="B160" s="2">
-        <v>2457326</v>
+        <v>2457296</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E160">
-        <v>57513217944</v>
+        <v>57513217937</v>
+      </c>
+      <c r="F160" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
@@ -3806,16 +3939,19 @@
         <v>165</v>
       </c>
       <c r="B161" s="2">
-        <v>2457342</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>41</v>
+        <v>2457318</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E161">
-        <v>57513217975</v>
+        <v>57513217951</v>
+      </c>
+      <c r="F161" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -3823,16 +3959,19 @@
         <v>165</v>
       </c>
       <c r="B162" s="2">
-        <v>2457288</v>
+        <v>2457326</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>166</v>
+        <v>7</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E162">
-        <v>57513217920</v>
+        <v>57513217944</v>
+      </c>
+      <c r="F162" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -3854,16 +3993,19 @@
         <v>165</v>
       </c>
       <c r="B164" s="2">
-        <v>2457318</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>42</v>
+        <v>2457342</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E164">
-        <v>57513217951</v>
+        <v>57513217975</v>
+      </c>
+      <c r="F164" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -3882,6 +4024,9 @@
       <c r="E165">
         <v>57513217968</v>
       </c>
+      <c r="F165" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
@@ -3919,41 +4064,47 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="B168" s="2">
-        <v>2438704</v>
+        <v>2145901</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>172</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>95</v>
+        <v>208</v>
+      </c>
+      <c r="E168" s="12">
+        <v>57513040214</v>
+      </c>
+      <c r="F168" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B169" s="2">
-        <v>2244790</v>
+        <v>2438704</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>42</v>
+        <v>172</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B170" s="2">
-        <v>2307898</v>
+        <v>2244790</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>8</v>
@@ -3961,13 +4112,13 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B171" s="2">
-        <v>443948</v>
+        <v>2307898</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>8</v>
@@ -3978,10 +4129,10 @@
         <v>175</v>
       </c>
       <c r="B172" s="2">
-        <v>789739</v>
+        <v>443948</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>8</v>
@@ -3989,22 +4140,16 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B173" s="2">
-        <v>594652</v>
+        <v>789739</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E173">
-        <v>628791004764</v>
-      </c>
-      <c r="F173" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -4020,7 +4165,7 @@
       <c r="D174" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E174">
+      <c r="E174" s="11">
         <v>628791004771</v>
       </c>
       <c r="F174" s="2">
@@ -4029,16 +4174,22 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B175" s="2">
-        <v>2370433</v>
+        <v>594652</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E175" s="7">
+        <v>628791004764</v>
+      </c>
+      <c r="F175" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
@@ -4046,24 +4197,30 @@
         <v>177</v>
       </c>
       <c r="B176" s="2">
-        <v>2391678</v>
+        <v>2370433</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E176" s="12">
+        <v>60752000789</v>
+      </c>
+      <c r="F176" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B177" s="2">
-        <v>2295695</v>
+        <v>2391678</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>8</v>
@@ -4074,55 +4231,74 @@
         <v>178</v>
       </c>
       <c r="B178" s="2">
-        <v>2295709</v>
+        <v>2295695</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E178">
+        <v>882936009353</v>
+      </c>
+      <c r="F178" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B179" s="2">
-        <v>2339617</v>
+        <v>2295709</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E179">
+        <v>882936009360</v>
+      </c>
+      <c r="F179" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B180" s="2">
-        <v>2421186</v>
+        <v>2339617</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E180" s="7"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B181" s="2">
-        <v>2463792</v>
+        <v>2421186</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="E181" s="9">
+        <v>63691073333</v>
+      </c>
+      <c r="F181" s="2">
+        <v>120</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -4130,7 +4306,7 @@
         <v>182</v>
       </c>
       <c r="B182" s="2">
-        <v>2463806</v>
+        <v>2463792</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>17</v>
@@ -4138,155 +4314,174 @@
       <c r="D182" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E182" s="9">
+        <v>63691082793</v>
+      </c>
+      <c r="F182" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B183" s="2">
-        <v>2450429</v>
+        <v>2463806</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
+      </c>
+      <c r="E183" s="9">
+        <v>63691082762</v>
+      </c>
+      <c r="F183" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="B184" s="2">
-        <v>2225964</v>
-      </c>
-      <c r="C184" s="2" t="s">
-        <v>42</v>
+        <v>2496003</v>
+      </c>
+      <c r="C184" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>33</v>
+        <v>206</v>
+      </c>
+      <c r="E184" s="12">
+        <v>63691100329</v>
+      </c>
+      <c r="F184" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B185" s="2">
+        <v>2450429</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D185" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" s="12">
+        <v>63691075764</v>
+      </c>
+      <c r="F185" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B186" s="2">
+        <v>2225964</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D186" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B187" s="2">
         <v>90800234</v>
       </c>
-      <c r="D185" s="2" t="s">
+      <c r="D187" s="2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B186" s="2">
-        <v>1913484</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E186">
-        <v>68510020406</v>
-      </c>
-      <c r="F186" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A187" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="B187" s="2">
-        <v>1913492</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E187" s="7">
-        <v>68510021403</v>
-      </c>
-      <c r="F187" s="2">
-        <v>100</v>
-      </c>
+      <c r="E187" s="7"/>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B188" s="2">
+        <v>1913484</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D188" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E188" s="11">
+        <v>68510020406</v>
+      </c>
+      <c r="F188" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B189" s="2">
+        <v>1913484</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D189" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E189" s="11">
+        <v>68510020802</v>
+      </c>
+      <c r="F189" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B190" s="2">
+        <v>1913492</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E190" s="11">
+        <v>68510021403</v>
+      </c>
+      <c r="F190" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B191" s="2">
         <v>2230584</v>
       </c>
-      <c r="C188" s="2" t="s">
+      <c r="C191" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D188" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E188">
+      <c r="D191" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191">
         <v>68510345400</v>
-      </c>
-      <c r="F188" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A189" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B189" s="2">
-        <v>2230585</v>
-      </c>
-      <c r="C189" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D189" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B190" s="2">
-        <v>2238334</v>
-      </c>
-      <c r="C190" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E190">
-        <v>68510899279</v>
-      </c>
-      <c r="F190" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B191" s="2">
-        <v>593435</v>
-      </c>
-      <c r="C191" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D191" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E191">
-        <v>64589001490</v>
       </c>
       <c r="F191" s="2">
         <v>100</v>
@@ -4294,93 +4489,93 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B192" s="2">
-        <v>593451</v>
+        <v>2230585</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>41</v>
+        <v>120</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E192">
-        <v>64589001575</v>
-      </c>
-      <c r="F192" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B193" s="2">
-        <v>2282941</v>
+        <v>2238334</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>168</v>
+        <v>27</v>
       </c>
       <c r="D193" s="2" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="E193">
-        <v>68510575128</v>
+        <v>68510899279</v>
       </c>
       <c r="F193" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B194" s="2">
-        <v>2282968</v>
+        <v>593435</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>170</v>
+        <v>42</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>66</v>
+        <v>8</v>
+      </c>
+      <c r="E194">
+        <v>64589001490</v>
+      </c>
+      <c r="F194" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B195" s="2">
-        <v>653241</v>
+        <v>593451</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>193</v>
+        <v>41</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E195">
-        <v>64589000752</v>
+        <v>64589001575</v>
       </c>
       <c r="F195" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="B196" s="2">
-        <v>653276</v>
+        <v>2053403</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>195</v>
+        <v>87</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E196">
-        <v>64589001643</v>
+        <v>56</v>
+      </c>
+      <c r="E196" s="12">
+        <v>64589002916</v>
       </c>
       <c r="F196" s="2">
         <v>500</v>
@@ -4388,137 +4583,139 @@
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B197" s="2">
-        <v>637742</v>
+        <v>2282941</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>35</v>
+        <v>168</v>
       </c>
       <c r="D197" s="2" t="s">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="E197">
+        <v>68510575128</v>
+      </c>
+      <c r="F197" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B198" s="2">
-        <v>637750</v>
+        <v>2282968</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>29</v>
+        <v>170</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="E198" s="7"/>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B199" s="2">
-        <v>711101</v>
+        <v>653241</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>23</v>
+        <v>193</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E199">
+        <v>64589000752</v>
+      </c>
+      <c r="F199" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B200" s="2">
-        <v>2302764</v>
+        <v>653276</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>42</v>
+        <v>195</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E200">
-        <v>68510801333</v>
+        <v>64589001643</v>
       </c>
       <c r="F200" s="2">
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B201" s="2">
-        <v>2302772</v>
+        <v>637742</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E201">
-        <v>68510802330</v>
-      </c>
-      <c r="F201" s="2">
-        <v>50</v>
-      </c>
+      <c r="E201" s="11"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B202" s="2">
-        <v>2302780</v>
+        <v>637750</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E202" s="7">
-        <v>771313162838</v>
-      </c>
-      <c r="F202" s="2">
-        <v>100</v>
-      </c>
+      <c r="E202" s="7"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B203" s="2">
-        <v>2384884</v>
+        <v>711101</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D203" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E203" s="7"/>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B204" s="2">
-        <v>2384892</v>
+        <v>2302764</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D204" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E204">
-        <v>68510181145</v>
+        <v>68510801333</v>
       </c>
       <c r="F204" s="2">
         <v>50</v>
@@ -4526,181 +4723,296 @@
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B205" s="2">
-        <v>2392925</v>
+        <v>2302772</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D205" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E205" s="11">
+        <v>68510802330</v>
+      </c>
+      <c r="F205" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B206" s="2">
-        <v>608165</v>
+        <v>2302780</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="D206" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E206">
-        <v>64589000561</v>
+      <c r="E206" s="11">
+        <v>771313162838</v>
       </c>
       <c r="F206" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B207" s="2">
-        <v>808571</v>
+        <v>2384884</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D207" s="2" t="s">
-        <v>8</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E207" s="11"/>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B208" s="2">
+        <v>2384892</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D208" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E208">
+        <v>68510181145</v>
+      </c>
+      <c r="F208" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B209" s="2">
+        <v>2392925</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D209" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B210" s="2">
+        <v>608165</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D210" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E210">
+        <v>64589000561</v>
+      </c>
+      <c r="F210" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B211" s="2">
+        <v>808571</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D211" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B208" s="2">
+      <c r="B212" s="2">
         <v>2163926</v>
       </c>
-      <c r="C208" s="2" t="s">
+      <c r="C212" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="D208" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A209" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B209" s="2">
-        <v>2322951</v>
-      </c>
-      <c r="C209" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A210" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B210" s="2">
-        <v>2322978</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A211" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B211" s="2">
-        <v>2347156</v>
-      </c>
-      <c r="C211" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A212" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B212" s="2">
-        <v>2347164</v>
-      </c>
-      <c r="C212" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D212" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B213" s="2">
-        <v>2347172</v>
+        <v>2322951</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E213">
+        <v>354092103102</v>
+      </c>
+      <c r="F213" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="2" t="s">
         <v>202</v>
       </c>
       <c r="B214" s="2">
+        <v>2322978</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D214" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E214">
+        <v>354092105106</v>
+      </c>
+      <c r="F214" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B215" s="2">
+        <v>2347156</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D215" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E215">
+        <v>354092102105</v>
+      </c>
+      <c r="F215" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B216" s="2">
+        <v>2347164</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D216" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E216">
+        <v>354092104109</v>
+      </c>
+      <c r="F216" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B217" s="2">
+        <v>2347172</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D217" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E217" s="7">
+        <v>354092106103</v>
+      </c>
+      <c r="F217" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B218" s="2">
         <v>2439603</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="C218" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D214" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A215" s="2" t="s">
+      <c r="D218" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E218" s="7">
+        <v>354092101313</v>
+      </c>
+      <c r="F218" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B215" s="2">
+      <c r="B219" s="2">
         <v>548359</v>
       </c>
-      <c r="C215" s="2" t="s">
+      <c r="C219" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D215" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A216" s="2" t="s">
+      <c r="D219" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E219" s="7"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B216" s="2">
+      <c r="B220" s="2">
         <v>548367</v>
       </c>
-      <c r="C216" s="2" t="s">
+      <c r="C220" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D216" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="D220" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" s="7"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F216">
-    <sortCondition ref="A2:A216"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F220">
+    <sortCondition ref="A2:A220"/>
+    <sortCondition ref="B2:B220"/>
+    <sortCondition ref="F2:F220"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Removing useless code, cleaning page
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B48ED76-B0D8-B248-BCB6-6866460A0B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E2F2BA-5F2F-CF4B-8105-FD14100E7386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1056,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F222" sqref="F222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
trying the din as key for the narc dictionnary:
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E2F2BA-5F2F-CF4B-8105-FD14100E7386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4162D5-08D4-0248-B523-5BBC7B470BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="209">
   <si>
     <t>Drug Name</t>
   </si>
@@ -632,9 +632,6 @@
   </si>
   <si>
     <t>XANAX</t>
-  </si>
-  <si>
-    <t>Act (if no upc use 1)</t>
   </si>
   <si>
     <t>TARO-TESTOSTERONE INJ</t>
@@ -734,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -745,11 +742,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F222" sqref="F222"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1091,45 +1086,44 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="8">
-        <v>1</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2439263</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>6</v>
+      <c r="A3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>2439263</v>
+        <v>2453908</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="2">
-        <v>2453908</v>
+        <v>2453916</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -1138,27 +1132,28 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2">
-        <v>2453916</v>
+        <v>2441969</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>2441969</v>
+        <v>2441934</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1166,24 +1161,24 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
-        <v>2441934</v>
+        <v>2249499</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
+      <c r="A8" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B8" s="2">
-        <v>2249499</v>
+        <v>2245345</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
@@ -1191,13 +1186,19 @@
       <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E8">
+        <v>55873030258</v>
+      </c>
+      <c r="F8" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="2">
-        <v>2245345</v>
+        <v>2245346</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
@@ -1206,7 +1207,7 @@
         <v>18</v>
       </c>
       <c r="E9">
-        <v>55873030258</v>
+        <v>55873030500</v>
       </c>
       <c r="F9" s="2">
         <v>30</v>
@@ -1214,22 +1215,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2">
-        <v>2245346</v>
+        <v>865397</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10">
-        <v>55873030500</v>
-      </c>
-      <c r="F10" s="2">
-        <v>30</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1237,67 +1232,73 @@
         <v>21</v>
       </c>
       <c r="B11" s="2">
-        <v>865397</v>
+        <v>865400</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E11">
+        <v>771313000253</v>
+      </c>
+      <c r="F11" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>21</v>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B12" s="2">
-        <v>865400</v>
+        <v>2177161</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E12">
-        <v>771313000253</v>
-      </c>
-      <c r="F12" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2">
-        <v>2177161</v>
+        <v>2244638</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E13">
+        <v>771313157285</v>
+      </c>
+      <c r="F13" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
-        <v>2244638</v>
+        <v>2177889</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E14">
-        <v>771313157285</v>
+        <v>771313078801</v>
       </c>
       <c r="F14" s="2">
-        <v>30</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1305,27 +1306,27 @@
         <v>28</v>
       </c>
       <c r="B15" s="2">
-        <v>2177889</v>
+        <v>2177897</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E15">
-        <v>771313078801</v>
+        <v>771313078702</v>
       </c>
       <c r="F15" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2">
-        <v>2177897</v>
+        <v>2364123</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>29</v>
@@ -1334,7 +1335,7 @@
         <v>8</v>
       </c>
       <c r="E16">
-        <v>771313078702</v>
+        <v>771313195836</v>
       </c>
       <c r="F16" s="2">
         <v>100</v>
@@ -1342,36 +1343,36 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B17" s="2">
-        <v>2364123</v>
+        <v>2476657</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17">
-        <v>771313195836</v>
-      </c>
-      <c r="F17" s="2">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2">
-        <v>2476657</v>
+        <v>655740</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>771313005487</v>
+      </c>
+      <c r="F18" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1379,19 +1380,19 @@
         <v>34</v>
       </c>
       <c r="B19" s="2">
-        <v>655740</v>
+        <v>655759</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E19">
-        <v>771313005487</v>
+        <v>771313258241</v>
       </c>
       <c r="F19" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1408,10 +1409,10 @@
         <v>8</v>
       </c>
       <c r="E20">
-        <v>771313258241</v>
+        <v>771313005524</v>
       </c>
       <c r="F20" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1419,41 +1420,41 @@
         <v>34</v>
       </c>
       <c r="B21" s="2">
-        <v>655759</v>
+        <v>655767</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E21">
-        <v>771313005524</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2">
-        <v>655767</v>
+        <v>2533669</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E22">
+        <v>771313253949</v>
+      </c>
+      <c r="F22" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2">
-        <v>2533669</v>
+        <v>2249324</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>27</v>
@@ -1462,7 +1463,7 @@
         <v>8</v>
       </c>
       <c r="E23">
-        <v>771313253949</v>
+        <v>771313162838</v>
       </c>
       <c r="F23" s="2">
         <v>100</v>
@@ -1470,22 +1471,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2">
-        <v>2249324</v>
+        <v>2330377</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E24">
-        <v>771313162838</v>
-      </c>
-      <c r="F24" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1493,10 +1488,10 @@
         <v>38</v>
       </c>
       <c r="B25" s="2">
-        <v>2330377</v>
+        <v>2452731</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>8</v>
@@ -1507,10 +1502,10 @@
         <v>38</v>
       </c>
       <c r="B26" s="2">
-        <v>2452731</v>
+        <v>2452758</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>8</v>
@@ -1518,16 +1513,22 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2">
-        <v>2452758</v>
+        <v>402680</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E27">
+        <v>771313006545</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1535,16 +1536,16 @@
         <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>402680</v>
+        <v>402737</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E28">
-        <v>771313006545</v>
+        <v>771313006606</v>
       </c>
       <c r="F28" s="2">
         <v>1000</v>
@@ -1555,16 +1556,16 @@
         <v>40</v>
       </c>
       <c r="B29" s="2">
-        <v>402737</v>
+        <v>402745</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E29">
-        <v>771313006606</v>
+        <v>771313006576</v>
       </c>
       <c r="F29" s="2">
         <v>1000</v>
@@ -1572,22 +1573,22 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B30" s="2">
-        <v>402745</v>
+        <v>2306530</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E30">
-        <v>771313006576</v>
+        <v>771313221757</v>
       </c>
       <c r="F30" s="2">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1595,19 +1596,13 @@
         <v>43</v>
       </c>
       <c r="B31" s="2">
-        <v>2306530</v>
+        <v>2366746</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E31">
-        <v>771313221757</v>
-      </c>
-      <c r="F31" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1615,10 +1610,10 @@
         <v>43</v>
       </c>
       <c r="B32" s="2">
-        <v>2366746</v>
+        <v>2366754</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>8</v>
@@ -1629,44 +1624,44 @@
         <v>43</v>
       </c>
       <c r="B33" s="2">
-        <v>2366754</v>
+        <v>2366762</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E33">
+        <v>771313221740</v>
+      </c>
+      <c r="F33" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2">
-        <v>2366762</v>
+        <v>2324628</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E34">
-        <v>771313221740</v>
-      </c>
-      <c r="F34" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B35" s="2">
-        <v>2324628</v>
+        <v>2426153</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>8</v>
@@ -1674,36 +1669,42 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B36" s="2">
-        <v>2426153</v>
+        <v>2336790</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E36">
+        <v>771313256360</v>
+      </c>
+      <c r="F36" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B37" s="2">
-        <v>2336790</v>
+        <v>2434946</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E37">
-        <v>771313256360</v>
+        <v>771313237703</v>
       </c>
       <c r="F37" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1711,30 +1712,24 @@
         <v>52</v>
       </c>
       <c r="B38" s="2">
-        <v>2434946</v>
+        <v>2436159</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E38">
-        <v>771313237703</v>
-      </c>
-      <c r="F38" s="2">
-        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B39" s="2">
-        <v>2436159</v>
+        <v>2041421</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>8</v>
@@ -1742,33 +1737,39 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B40" s="2">
-        <v>2041421</v>
+        <v>50024</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
+      </c>
+      <c r="E40" s="9">
+        <v>68625100253</v>
+      </c>
+      <c r="F40" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B41" s="2">
-        <v>50024</v>
+        <v>380571</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="9">
-        <v>68625100253</v>
+      <c r="E41" s="7">
+        <v>68625100352</v>
       </c>
       <c r="F41" s="2">
         <v>500</v>
@@ -1776,39 +1777,39 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B42" s="2">
-        <v>380571</v>
+        <v>2479672</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="9">
-        <v>68625100352</v>
+        <v>8</v>
+      </c>
+      <c r="E42" s="7">
+        <v>886965005492</v>
       </c>
       <c r="F42" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" s="2">
-        <v>2479672</v>
+        <v>2439050</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E43">
-        <v>886965005492</v>
+      <c r="E43" s="9">
+        <v>886965002392</v>
       </c>
       <c r="F43" s="2">
         <v>100</v>
@@ -1816,19 +1817,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" s="2">
-        <v>2439050</v>
+        <v>2277131</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E44">
-        <v>886965002392</v>
+        <v>60025101151</v>
       </c>
       <c r="F44" s="2">
         <v>100</v>
@@ -1839,16 +1840,16 @@
         <v>61</v>
       </c>
       <c r="B45" s="2">
-        <v>2277131</v>
+        <v>2277158</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E45">
-        <v>60025101151</v>
+        <v>60025101205</v>
       </c>
       <c r="F45" s="2">
         <v>100</v>
@@ -1859,16 +1860,16 @@
         <v>61</v>
       </c>
       <c r="B46" s="2">
-        <v>2277158</v>
+        <v>2277166</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E46">
-        <v>60025101205</v>
+        <v>60025101007</v>
       </c>
       <c r="F46" s="2">
         <v>100</v>
@@ -1879,16 +1880,16 @@
         <v>61</v>
       </c>
       <c r="B47" s="2">
-        <v>2277166</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>27</v>
+        <v>2277174</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E47">
-        <v>60025101007</v>
+        <v>60025101304</v>
       </c>
       <c r="F47" s="2">
         <v>100</v>
@@ -1899,16 +1900,16 @@
         <v>61</v>
       </c>
       <c r="B48" s="2">
-        <v>2277174</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>41</v>
+        <v>2277182</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="11">
-        <v>60025101304</v>
+      <c r="E48">
+        <v>60025101403</v>
       </c>
       <c r="F48" s="2">
         <v>100</v>
@@ -1919,17 +1920,15 @@
         <v>61</v>
       </c>
       <c r="B49" s="2">
-        <v>2277182</v>
+        <v>2277204</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E49">
-        <v>60025101403</v>
-      </c>
+      <c r="E49" s="9"/>
       <c r="F49" s="2">
         <v>100</v>
       </c>
@@ -1939,10 +1938,10 @@
         <v>61</v>
       </c>
       <c r="B50" s="2">
-        <v>2277204</v>
+        <v>2277212</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>33</v>
@@ -1954,51 +1953,48 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B51" s="2">
-        <v>2277212</v>
+        <v>2450771</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="E51" s="7">
+        <v>60025418891</v>
+      </c>
       <c r="F51" s="2">
-        <v>100</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B52" s="2">
-        <v>2450771</v>
+        <v>2341220</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="7">
-        <v>60025418891</v>
-      </c>
-      <c r="F52" s="2">
-        <v>4</v>
-      </c>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B53" s="2">
-        <v>2341220</v>
+        <v>2341174</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>66</v>
@@ -2007,51 +2003,51 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B54" s="2">
-        <v>2341174</v>
+        <v>535230</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E54" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="E54" s="7">
+        <v>64589001889</v>
+      </c>
+      <c r="F54" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B55" s="2">
-        <v>535230</v>
+        <v>2172917</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E55" s="7">
-        <v>64589001889</v>
-      </c>
-      <c r="F55" s="2">
-        <v>100</v>
-      </c>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B56" s="2">
-        <v>2172917</v>
+        <v>548375</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="E56" s="7"/>
     </row>
@@ -2060,10 +2056,10 @@
         <v>75</v>
       </c>
       <c r="B57" s="2">
-        <v>548375</v>
+        <v>2256193</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>33</v>
@@ -2072,13 +2068,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B58" s="2">
-        <v>2256193</v>
+        <v>618454</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>33</v>
@@ -2087,13 +2083,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B59" s="2">
-        <v>618454</v>
+        <v>860689</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>33</v>
@@ -2105,10 +2101,10 @@
         <v>78</v>
       </c>
       <c r="B60" s="2">
-        <v>860689</v>
+        <v>860697</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>33</v>
@@ -2120,10 +2116,10 @@
         <v>78</v>
       </c>
       <c r="B61" s="2">
-        <v>860697</v>
+        <v>860700</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>33</v>
@@ -2132,34 +2128,39 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B62" s="2">
-        <v>860700</v>
+        <v>2247732</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E62" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E62" s="7">
+        <v>62773610558</v>
+      </c>
+      <c r="F62" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B63" s="2">
-        <v>2247732</v>
+        <v>2247733</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E63" s="7">
-        <v>62773610558</v>
+        <v>62773610565</v>
       </c>
       <c r="F63" s="2">
         <v>100</v>
@@ -2170,16 +2171,16 @@
         <v>81</v>
       </c>
       <c r="B64" s="2">
-        <v>2247733</v>
+        <v>2247734</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>82</v>
+        <v>13</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E64" s="7">
-        <v>62773610565</v>
+        <v>62773610572</v>
       </c>
       <c r="F64" s="2">
         <v>100</v>
@@ -2190,16 +2191,16 @@
         <v>81</v>
       </c>
       <c r="B65" s="2">
-        <v>2247734</v>
+        <v>2250241</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="7">
-        <v>62773610572</v>
+        <v>62773610824</v>
       </c>
       <c r="F65" s="2">
         <v>100</v>
@@ -2207,110 +2208,105 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B66" s="2">
-        <v>2250241</v>
+        <v>2224577</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E66" s="7">
-        <v>62773610824</v>
-      </c>
-      <c r="F66" s="2">
-        <v>100</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B67" s="2">
-        <v>2224577</v>
+        <v>2230769</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="E67" s="7">
+        <v>775848181005</v>
+      </c>
+      <c r="F67" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B68" s="2">
-        <v>2230769</v>
+        <v>29246</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E68" s="7">
-        <v>775848181005</v>
-      </c>
-      <c r="F68" s="2">
-        <v>500</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B69" s="2">
-        <v>29246</v>
+        <v>2138018</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B70" s="2">
-        <v>2138018</v>
+        <v>30783</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B71" s="2">
-        <v>30783</v>
+        <v>1924516</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B72" s="2">
-        <v>1924516</v>
+        <v>2443236</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>44</v>
@@ -2318,14 +2314,19 @@
       <c r="D72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="7"/>
+      <c r="E72" s="7">
+        <v>660933002535</v>
+      </c>
+      <c r="F72" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B73" s="2">
-        <v>2443236</v>
+        <v>362158</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>44</v>
@@ -2334,7 +2335,7 @@
         <v>8</v>
       </c>
       <c r="E73" s="7">
-        <v>660933002535</v>
+        <v>660933002603</v>
       </c>
       <c r="F73" s="2">
         <v>100</v>
@@ -2345,16 +2346,16 @@
         <v>98</v>
       </c>
       <c r="B74" s="2">
-        <v>362158</v>
+        <v>405329</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E74" s="7">
-        <v>660933002603</v>
+        <v>660933002597</v>
       </c>
       <c r="F74" s="2">
         <v>100</v>
@@ -2365,16 +2366,16 @@
         <v>98</v>
       </c>
       <c r="B75" s="2">
-        <v>405329</v>
+        <v>405337</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E75" s="7">
-        <v>660933002597</v>
+        <v>660933002610</v>
       </c>
       <c r="F75" s="2">
         <v>100</v>
@@ -2382,19 +2383,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B76" s="2">
-        <v>405337</v>
+        <v>125083</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="7">
-        <v>660933002610</v>
+        <v>60025405952</v>
       </c>
       <c r="F76" s="2">
         <v>100</v>
@@ -2405,16 +2406,16 @@
         <v>99</v>
       </c>
       <c r="B77" s="2">
-        <v>125083</v>
+        <v>125121</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E77" s="7">
-        <v>60025405952</v>
+        <v>60025405976</v>
       </c>
       <c r="F77" s="2">
         <v>100</v>
@@ -2425,16 +2426,16 @@
         <v>99</v>
       </c>
       <c r="B78" s="2">
-        <v>125121</v>
+        <v>705438</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E78" s="7">
-        <v>60025405976</v>
+        <v>60025405938</v>
       </c>
       <c r="F78" s="2">
         <v>100</v>
@@ -2445,45 +2446,40 @@
         <v>99</v>
       </c>
       <c r="B79" s="2">
-        <v>705438</v>
+        <v>786543</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="7">
-        <v>60025405938</v>
-      </c>
-      <c r="F79" s="2">
-        <v>100</v>
-      </c>
+      <c r="E79" s="7"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B80" s="2">
-        <v>786543</v>
+        <v>2244080</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E80" s="7"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B81" s="2">
-        <v>2244080</v>
+        <v>614491</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>56</v>
@@ -2492,27 +2488,27 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B82" s="2">
-        <v>614491</v>
+        <v>226327</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B83" s="2">
-        <v>226327</v>
+        <v>176206</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>33</v>
@@ -2520,13 +2516,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B84" s="2">
-        <v>176206</v>
+        <v>176192</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>33</v>
@@ -2534,36 +2530,42 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B85" s="2">
-        <v>176192</v>
+        <v>521698</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E85">
+        <v>660933001866</v>
+      </c>
+      <c r="F85" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B86" s="2">
-        <v>521698</v>
+        <v>2470292</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E86">
-        <v>660933001866</v>
+        <v>60025422034</v>
       </c>
       <c r="F86" s="2">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -2571,16 +2573,16 @@
         <v>113</v>
       </c>
       <c r="B87" s="2">
-        <v>2470292</v>
+        <v>2470306</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E87">
-        <v>60025422034</v>
+        <v>60025422041</v>
       </c>
       <c r="F87" s="2">
         <v>60</v>
@@ -2591,16 +2593,16 @@
         <v>113</v>
       </c>
       <c r="B88" s="2">
-        <v>2470306</v>
+        <v>2470314</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E88">
-        <v>60025422041</v>
+        <v>60025422058</v>
       </c>
       <c r="F88" s="2">
         <v>60</v>
@@ -2611,16 +2613,16 @@
         <v>113</v>
       </c>
       <c r="B89" s="2">
-        <v>2470314</v>
+        <v>2470322</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E89">
-        <v>60025422058</v>
+        <v>60025422065</v>
       </c>
       <c r="F89" s="2">
         <v>60</v>
@@ -2628,36 +2630,36 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B90" s="2">
-        <v>2470322</v>
+        <v>1916580</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E90">
-        <v>60025422065</v>
-      </c>
-      <c r="F90" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B91" s="2">
-        <v>1916580</v>
+        <v>2125323</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>105</v>
+        <v>25</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>56</v>
+        <v>33</v>
+      </c>
+      <c r="E91">
+        <v>60025409523</v>
+      </c>
+      <c r="F91" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
@@ -2665,16 +2667,16 @@
         <v>119</v>
       </c>
       <c r="B92" s="2">
-        <v>2125323</v>
+        <v>2125331</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E92">
-        <v>60025409523</v>
+        <v>60025409530</v>
       </c>
       <c r="F92" s="2">
         <v>60</v>
@@ -2685,16 +2687,16 @@
         <v>119</v>
       </c>
       <c r="B93" s="2">
-        <v>2125331</v>
+        <v>2125366</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E93">
-        <v>60025409530</v>
+        <v>60025409547</v>
       </c>
       <c r="F93" s="2">
         <v>60</v>
@@ -2705,16 +2707,16 @@
         <v>119</v>
       </c>
       <c r="B94" s="2">
-        <v>2125366</v>
+        <v>2125382</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E94">
-        <v>60025409547</v>
+        <v>60025409561</v>
       </c>
       <c r="F94" s="2">
         <v>60</v>
@@ -2725,16 +2727,16 @@
         <v>119</v>
       </c>
       <c r="B95" s="2">
-        <v>2125382</v>
+        <v>2125390</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>121</v>
+        <v>41</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E95">
-        <v>60025409561</v>
+        <v>60025409578</v>
       </c>
       <c r="F95" s="2">
         <v>60</v>
@@ -2745,16 +2747,16 @@
         <v>119</v>
       </c>
       <c r="B96" s="2">
-        <v>2125390</v>
+        <v>2359510</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E96">
-        <v>60025409578</v>
+        <v>60025410598</v>
       </c>
       <c r="F96" s="2">
         <v>60</v>
@@ -2762,56 +2764,56 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B97" s="2">
-        <v>2359510</v>
+        <v>2388308</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E97">
-        <v>60025410598</v>
+        <v>622082288376</v>
       </c>
       <c r="F97" s="2">
-        <v>60</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B98" s="2">
-        <v>2388308</v>
+        <v>2400111</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E98">
-        <v>622082288376</v>
-      </c>
-      <c r="F98" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B99" s="2">
-        <v>2400111</v>
+        <v>2184435</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E99">
+        <v>55873100104</v>
+      </c>
+      <c r="F99" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -2819,16 +2821,16 @@
         <v>125</v>
       </c>
       <c r="B100" s="2">
-        <v>2184435</v>
+        <v>2184443</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E100">
-        <v>55873100104</v>
+        <v>55873100111</v>
       </c>
       <c r="F100" s="2">
         <v>100</v>
@@ -2839,19 +2841,19 @@
         <v>125</v>
       </c>
       <c r="B101" s="2">
-        <v>2184443</v>
+        <v>2184451</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E101">
-        <v>55873100111</v>
+        <v>55873100128</v>
       </c>
       <c r="F101" s="2">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -2859,30 +2861,24 @@
         <v>125</v>
       </c>
       <c r="B102" s="2">
-        <v>2184451</v>
+        <v>2242163</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>126</v>
+        <v>27</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E102">
-        <v>55873100128</v>
-      </c>
-      <c r="F102" s="2">
-        <v>50</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B103" s="2">
-        <v>2242163</v>
+        <v>115630</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>33</v>
@@ -2890,36 +2886,42 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B104" s="2">
-        <v>115630</v>
+        <v>36323</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E104">
+        <v>55860010157</v>
+      </c>
+      <c r="F104" s="2">
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B105" s="2">
-        <v>36323</v>
+        <v>2410745</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>129</v>
+        <v>23</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E105">
-        <v>55860010157</v>
+        <v>660933002313</v>
       </c>
       <c r="F105" s="2">
-        <v>250</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
@@ -2927,16 +2929,16 @@
         <v>130</v>
       </c>
       <c r="B106" s="2">
-        <v>2410745</v>
+        <v>2410753</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E106">
-        <v>660933002313</v>
+        <v>660933002320</v>
       </c>
       <c r="F106" s="2">
         <v>100</v>
@@ -2944,36 +2946,36 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B107" s="2">
-        <v>2410753</v>
+        <v>2410761</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E107">
-        <v>660933002320</v>
-      </c>
-      <c r="F107" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B108" s="2">
-        <v>2410761</v>
+        <v>2019930</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E108">
+        <v>871547000859</v>
+      </c>
+      <c r="F108" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
@@ -2981,16 +2983,16 @@
         <v>132</v>
       </c>
       <c r="B109" s="2">
-        <v>2019930</v>
+        <v>2019949</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E109">
-        <v>871547000859</v>
+        <v>871547000897</v>
       </c>
       <c r="F109" s="2">
         <v>50</v>
@@ -3001,16 +3003,16 @@
         <v>132</v>
       </c>
       <c r="B110" s="2">
-        <v>2019949</v>
+        <v>2019957</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E110">
-        <v>871547000897</v>
+        <v>871547000910</v>
       </c>
       <c r="F110" s="2">
         <v>50</v>
@@ -3021,19 +3023,13 @@
         <v>132</v>
       </c>
       <c r="B111" s="2">
-        <v>2019957</v>
+        <v>2019965</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E111">
-        <v>871547000910</v>
-      </c>
-      <c r="F111" s="2">
-        <v>50</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -3041,53 +3037,53 @@
         <v>132</v>
       </c>
       <c r="B112" s="2">
-        <v>2019965</v>
+        <v>2177749</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E112">
+        <v>871547000873</v>
+      </c>
+      <c r="F112" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B113" s="2">
-        <v>2177749</v>
+        <v>2480859</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E113">
-        <v>871547000873</v>
+        <v>697359005734</v>
       </c>
       <c r="F113" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B114" s="2">
-        <v>2480859</v>
+        <v>2247699</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E114">
-        <v>697359005734</v>
-      </c>
-      <c r="F114" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -3095,115 +3091,121 @@
         <v>134</v>
       </c>
       <c r="B115" s="2">
-        <v>2247699</v>
+        <v>2247700</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E115">
+        <v>628791004627</v>
+      </c>
+      <c r="F115" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B116" s="2">
-        <v>2247700</v>
+        <v>2394618</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E116">
-        <v>628791004627</v>
+        <v>95</v>
+      </c>
+      <c r="E116" s="9">
+        <v>30406000304</v>
       </c>
       <c r="F116" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B117" s="2">
-        <v>2394618</v>
+        <v>511528</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>136</v>
+        <v>44</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E117" s="9">
-        <v>30406000304</v>
+        <v>8</v>
+      </c>
+      <c r="E117" s="7">
+        <v>660933001712</v>
       </c>
       <c r="F117" s="2">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B118" s="2">
-        <v>511528</v>
+        <v>2474980</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E118">
-        <v>660933001712</v>
-      </c>
-      <c r="F118" s="2">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B119" s="2">
-        <v>2474980</v>
+        <v>2137534</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>136</v>
+        <v>22</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B120" s="2">
-        <v>2137534</v>
+        <v>2049481</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B121" s="2">
-        <v>2049481</v>
+        <v>2378272</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>141</v>
+        <v>49</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>56</v>
+        <v>8</v>
+      </c>
+      <c r="E121">
+        <v>628791006294</v>
+      </c>
+      <c r="F121" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -3219,22 +3221,16 @@
       <c r="D122" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E122">
-        <v>628791006294</v>
-      </c>
-      <c r="F122" s="2">
-        <v>100</v>
-      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B123" s="2">
-        <v>2378272</v>
+        <v>2372533</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>8</v>
@@ -3245,10 +3241,10 @@
         <v>143</v>
       </c>
       <c r="B124" s="2">
-        <v>2372533</v>
+        <v>2372568</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>8</v>
@@ -3259,53 +3255,59 @@
         <v>143</v>
       </c>
       <c r="B125" s="2">
-        <v>2372568</v>
+        <v>2372797</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E125">
+        <v>60025409844</v>
+      </c>
+      <c r="F125" s="2">
+        <v>60</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B126" s="2">
-        <v>2372797</v>
+        <v>2324253</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E126">
-        <v>60025409844</v>
+        <v>625972019869</v>
       </c>
       <c r="F126" s="2">
-        <v>60</v>
+        <v>500</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="2" t="s">
-        <v>144</v>
+      <c r="A127" s="4" t="s">
+        <v>145</v>
       </c>
       <c r="B127" s="2">
-        <v>2324253</v>
+        <v>2424851</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E127">
-        <v>625972019869</v>
+        <v>57606111340</v>
       </c>
       <c r="F127" s="2">
-        <v>500</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -3313,39 +3315,33 @@
         <v>145</v>
       </c>
       <c r="B128" s="2">
-        <v>2424851</v>
+        <v>2424878</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E128">
-        <v>57606111340</v>
+        <v>57606111357</v>
       </c>
       <c r="F128" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="4" t="s">
-        <v>145</v>
+      <c r="A129" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="B129" s="2">
-        <v>2424878</v>
+        <v>2048701</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E129">
-        <v>57606111357</v>
-      </c>
-      <c r="F129" s="2">
-        <v>30</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -3353,13 +3349,19 @@
         <v>146</v>
       </c>
       <c r="B130" s="2">
-        <v>2048701</v>
+        <v>2048728</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E130">
+        <v>57606872821</v>
+      </c>
+      <c r="F130" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -3367,16 +3369,16 @@
         <v>146</v>
       </c>
       <c r="B131" s="2">
-        <v>2048728</v>
+        <v>2048736</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E131">
-        <v>57606872821</v>
+        <v>57606873620</v>
       </c>
       <c r="F131" s="2">
         <v>100</v>
@@ -3384,19 +3386,19 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B132" s="2">
-        <v>2048736</v>
+        <v>2207818</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E132">
-        <v>57606873620</v>
+        <v>57606781826</v>
       </c>
       <c r="F132" s="2">
         <v>100</v>
@@ -3416,30 +3418,30 @@
         <v>8</v>
       </c>
       <c r="E133">
-        <v>57606781826</v>
+        <v>57606781840</v>
       </c>
       <c r="F133" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B134" s="2">
-        <v>2207818</v>
+        <v>885401</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E134">
-        <v>57606781840</v>
+        <v>57606540140</v>
       </c>
       <c r="F134" s="2">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -3447,16 +3449,16 @@
         <v>148</v>
       </c>
       <c r="B135" s="2">
-        <v>885401</v>
+        <v>885428</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E135">
-        <v>57606540140</v>
+        <v>57606542847</v>
       </c>
       <c r="F135" s="2">
         <v>100</v>
@@ -3467,16 +3469,16 @@
         <v>148</v>
       </c>
       <c r="B136" s="2">
-        <v>885428</v>
+        <v>885436</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E136">
-        <v>57606542847</v>
+        <v>57606543646</v>
       </c>
       <c r="F136" s="2">
         <v>100</v>
@@ -3487,16 +3489,16 @@
         <v>148</v>
       </c>
       <c r="B137" s="2">
-        <v>885436</v>
+        <v>885444</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E137">
-        <v>57606543646</v>
+        <v>57606544445</v>
       </c>
       <c r="F137" s="2">
         <v>100</v>
@@ -3504,36 +3506,36 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B138" s="2">
-        <v>885444</v>
+        <v>1916386</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E138">
-        <v>57606544445</v>
-      </c>
-      <c r="F138" s="2">
-        <v>100</v>
+        <v>56</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B139" s="2">
-        <v>1916386</v>
+        <v>728187</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>105</v>
+        <v>23</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>56</v>
+        <v>8</v>
+      </c>
+      <c r="E139">
+        <v>57606818720</v>
+      </c>
+      <c r="F139" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -3541,16 +3543,16 @@
         <v>150</v>
       </c>
       <c r="B140" s="2">
-        <v>728187</v>
+        <v>728195</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E140">
-        <v>57606818720</v>
+        <v>57606819529</v>
       </c>
       <c r="F140" s="2">
         <v>100</v>
@@ -3561,16 +3563,16 @@
         <v>150</v>
       </c>
       <c r="B141" s="2">
-        <v>728195</v>
+        <v>728209</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E141">
-        <v>57606819529</v>
+        <v>57606820921</v>
       </c>
       <c r="F141" s="2">
         <v>100</v>
@@ -3578,36 +3580,30 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B142" s="2">
-        <v>728209</v>
+        <v>584991</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E142">
-        <v>57606820921</v>
-      </c>
-      <c r="F142" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B143" s="2">
-        <v>584991</v>
+        <v>2380897</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -3615,31 +3611,36 @@
         <v>152</v>
       </c>
       <c r="B144" s="2">
-        <v>2380897</v>
+        <v>2380900</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E144" s="11"/>
+      <c r="E144" s="9">
+        <v>57606022479</v>
+      </c>
+      <c r="F144" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B145" s="2">
-        <v>2380900</v>
+        <v>2380919</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E145" s="7">
-        <v>57606022479</v>
+        <v>57606022493</v>
       </c>
       <c r="F145" s="2">
         <v>100</v>
@@ -3647,30 +3648,25 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B146" s="2">
-        <v>2380919</v>
+        <v>2319977</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E146" s="7">
-        <v>57606022493</v>
-      </c>
-      <c r="F146" s="2">
-        <v>100</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E146" s="7"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B147" s="2">
-        <v>2319977</v>
+        <v>2436175</v>
       </c>
       <c r="C147" s="2" t="s">
         <v>44</v>
@@ -3678,80 +3674,86 @@
       <c r="D147" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E147" s="7"/>
+      <c r="E147" s="7">
+        <v>57606025876</v>
+      </c>
+      <c r="F147" s="2">
+        <v>30</v>
+      </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B148" s="2">
-        <v>2436175</v>
+        <v>2436183</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E148" s="9">
-        <v>57606025876</v>
-      </c>
-      <c r="F148" s="2">
-        <v>30</v>
-      </c>
+      <c r="E148" s="7"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B149" s="2">
-        <v>2436183</v>
+        <v>2299216</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>27</v>
+        <v>156</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E149">
+        <v>60752140157</v>
+      </c>
+      <c r="F149" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B150" s="2">
-        <v>2299216</v>
+        <v>608882</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E150">
-        <v>60752140157</v>
+        <v>64589001599</v>
       </c>
       <c r="F150" s="2">
-        <v>90</v>
+        <v>500</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B151" s="2">
-        <v>608882</v>
+        <v>653233</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E151">
-        <v>64589001599</v>
+        <v>64589002138</v>
       </c>
       <c r="F151" s="2">
-        <v>500</v>
+        <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -3768,27 +3770,27 @@
         <v>33</v>
       </c>
       <c r="E152">
-        <v>64589002138</v>
+        <v>64589001926</v>
       </c>
       <c r="F152" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B153" s="2">
-        <v>653233</v>
+        <v>608238</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="D153" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E153">
-        <v>64589001926</v>
+      <c r="E153" s="9">
+        <v>64589000936</v>
       </c>
       <c r="F153" s="2">
         <v>100</v>
@@ -3796,19 +3798,19 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B154" s="2">
-        <v>608238</v>
+        <v>608181</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D154" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E154" s="9">
-        <v>64589000936</v>
+      <c r="E154" s="7">
+        <v>64589002305</v>
       </c>
       <c r="F154" s="2">
         <v>100</v>
@@ -3816,19 +3818,19 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B155" s="2">
-        <v>608181</v>
+        <v>608203</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D155" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E155" s="9">
-        <v>64589002305</v>
+      <c r="E155" s="7">
+        <v>64589002299</v>
       </c>
       <c r="F155" s="2">
         <v>100</v>
@@ -3836,19 +3838,19 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B156" s="2">
-        <v>608203</v>
+        <v>604453</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="D156" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E156" s="9">
-        <v>64589002299</v>
+      <c r="E156" s="7">
+        <v>660933002047</v>
       </c>
       <c r="F156" s="2">
         <v>100</v>
@@ -3859,16 +3861,16 @@
         <v>164</v>
       </c>
       <c r="B157" s="2">
-        <v>604453</v>
+        <v>604461</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D157" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E157">
-        <v>660933002047</v>
+        <v>660933002054</v>
       </c>
       <c r="F157" s="2">
         <v>100</v>
@@ -3876,19 +3878,19 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B158" s="2">
-        <v>604461</v>
+        <v>2457288</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>41</v>
+        <v>166</v>
       </c>
       <c r="D158" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E158">
-        <v>660933002054</v>
+        <v>57513217920</v>
       </c>
       <c r="F158" s="2">
         <v>100</v>
@@ -3899,16 +3901,16 @@
         <v>165</v>
       </c>
       <c r="B159" s="2">
-        <v>2457288</v>
+        <v>2457296</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="D159" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E159">
-        <v>57513217920</v>
+        <v>57513217937</v>
       </c>
       <c r="F159" s="2">
         <v>100</v>
@@ -3919,16 +3921,16 @@
         <v>165</v>
       </c>
       <c r="B160" s="2">
-        <v>2457296</v>
-      </c>
-      <c r="C160" s="2" t="s">
-        <v>27</v>
+        <v>2457318</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D160" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E160">
-        <v>57513217937</v>
+        <v>57513217951</v>
       </c>
       <c r="F160" s="2">
         <v>100</v>
@@ -3939,16 +3941,16 @@
         <v>165</v>
       </c>
       <c r="B161" s="2">
-        <v>2457318</v>
-      </c>
-      <c r="C161" s="5" t="s">
-        <v>42</v>
+        <v>2457326</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="D161" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E161">
-        <v>57513217951</v>
+        <v>57513217944</v>
       </c>
       <c r="F161" s="2">
         <v>100</v>
@@ -3959,19 +3961,13 @@
         <v>165</v>
       </c>
       <c r="B162" s="2">
-        <v>2457326</v>
+        <v>2457334</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>7</v>
+        <v>114</v>
       </c>
       <c r="D162" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E162">
-        <v>57513217944</v>
-      </c>
-      <c r="F162" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -3979,13 +3975,19 @@
         <v>165</v>
       </c>
       <c r="B163" s="2">
-        <v>2457334</v>
+        <v>2457342</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>114</v>
+        <v>41</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E163">
+        <v>57513217975</v>
+      </c>
+      <c r="F163" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
@@ -3993,16 +3995,16 @@
         <v>165</v>
       </c>
       <c r="B164" s="2">
-        <v>2457342</v>
+        <v>2457344</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>41</v>
+        <v>114</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E164">
-        <v>57513217975</v>
+        <v>57513217968</v>
       </c>
       <c r="F164" s="2">
         <v>100</v>
@@ -4010,101 +4012,95 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B165" s="2">
-        <v>2457344</v>
+        <v>2327120</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="E165">
-        <v>57513217968</v>
+        <v>57513141904</v>
       </c>
       <c r="F165" s="2">
-        <v>100</v>
+        <v>5</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B166" s="2">
-        <v>2327120</v>
+        <v>2327147</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D166" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E166">
-        <v>57513141904</v>
-      </c>
-      <c r="F166" s="2">
-        <v>5</v>
-      </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>169</v>
+        <v>208</v>
       </c>
       <c r="B167" s="2">
-        <v>2327147</v>
+        <v>2145901</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>66</v>
+        <v>207</v>
+      </c>
+      <c r="E167">
+        <v>57513040214</v>
+      </c>
+      <c r="F167" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="B168" s="2">
-        <v>2145901</v>
+        <v>2438704</v>
       </c>
       <c r="C168" s="2" t="s">
         <v>172</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E168" s="12">
-        <v>57513040214</v>
-      </c>
-      <c r="F168" s="2">
-        <v>10</v>
+        <v>95</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B169" s="2">
-        <v>2438704</v>
+        <v>2244790</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B170" s="2">
-        <v>2244790</v>
+        <v>2307898</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>8</v>
@@ -4112,13 +4108,13 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B171" s="2">
-        <v>2307898</v>
+        <v>443948</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>8</v>
@@ -4129,10 +4125,10 @@
         <v>175</v>
       </c>
       <c r="B172" s="2">
-        <v>443948</v>
+        <v>789739</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>8</v>
@@ -4140,16 +4136,22 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B173" s="2">
-        <v>789739</v>
+        <v>594644</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E173">
+        <v>628791004771</v>
+      </c>
+      <c r="F173" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -4157,16 +4159,16 @@
         <v>176</v>
       </c>
       <c r="B174" s="2">
-        <v>594644</v>
+        <v>594652</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E174" s="11">
-        <v>628791004771</v>
+      <c r="E174" s="9">
+        <v>628791004764</v>
       </c>
       <c r="F174" s="2">
         <v>100</v>
@@ -4174,22 +4176,22 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B175" s="2">
-        <v>594652</v>
+        <v>2370433</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D175" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E175" s="7">
-        <v>628791004764</v>
+        <v>60752000789</v>
       </c>
       <c r="F175" s="2">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
@@ -4197,33 +4199,33 @@
         <v>177</v>
       </c>
       <c r="B176" s="2">
-        <v>2370433</v>
+        <v>2391678</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E176" s="12">
-        <v>60752000789</v>
-      </c>
-      <c r="F176" s="2">
-        <v>30</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B177" s="2">
-        <v>2391678</v>
+        <v>2295695</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E177">
+        <v>882936009353</v>
+      </c>
+      <c r="F177" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -4231,16 +4233,16 @@
         <v>178</v>
       </c>
       <c r="B178" s="2">
-        <v>2295695</v>
+        <v>2295709</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E178">
-        <v>882936009353</v>
+        <v>882936009360</v>
       </c>
       <c r="F178" s="2">
         <v>28</v>
@@ -4248,57 +4250,57 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B179" s="2">
-        <v>2295709</v>
+        <v>2339617</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E179">
-        <v>882936009360</v>
-      </c>
-      <c r="F179" s="2">
-        <v>28</v>
-      </c>
+      <c r="E179" s="9"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B180" s="2">
-        <v>2339617</v>
+        <v>2421186</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>180</v>
+        <v>45</v>
       </c>
       <c r="D180" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E180" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="E180" s="7">
+        <v>63691073333</v>
+      </c>
+      <c r="F180" s="2">
+        <v>120</v>
+      </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B181" s="2">
-        <v>2421186</v>
+        <v>2463792</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D181" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E181" s="9">
-        <v>63691073333</v>
+        <v>18</v>
+      </c>
+      <c r="E181" s="7">
+        <v>63691082793</v>
       </c>
       <c r="F181" s="2">
-        <v>120</v>
+        <v>30</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
@@ -4306,7 +4308,7 @@
         <v>182</v>
       </c>
       <c r="B182" s="2">
-        <v>2463792</v>
+        <v>2463806</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>17</v>
@@ -4314,8 +4316,8 @@
       <c r="D182" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E182" s="9">
-        <v>63691082793</v>
+      <c r="E182" s="7">
+        <v>63691082762</v>
       </c>
       <c r="F182" s="2">
         <v>30</v>
@@ -4323,19 +4325,19 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
-        <v>182</v>
+        <v>204</v>
       </c>
       <c r="B183" s="2">
-        <v>2463806</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>17</v>
+        <v>2496003</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="D183" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E183" s="9">
-        <v>63691082762</v>
+        <v>205</v>
+      </c>
+      <c r="E183" s="7">
+        <v>63691100329</v>
       </c>
       <c r="F183" s="2">
         <v>30</v>
@@ -4343,69 +4345,69 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="B184" s="2">
-        <v>2496003</v>
-      </c>
-      <c r="C184" s="10" t="s">
-        <v>94</v>
+        <v>2450429</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="D184" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E184" s="12">
-        <v>63691100329</v>
+        <v>8</v>
+      </c>
+      <c r="E184">
+        <v>63691075764</v>
       </c>
       <c r="F184" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B185" s="2">
-        <v>2450429</v>
+        <v>2225964</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>126</v>
+        <v>42</v>
       </c>
       <c r="D185" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E185" s="12">
-        <v>63691075764</v>
-      </c>
-      <c r="F185" s="2">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B186" s="2">
-        <v>2225964</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>42</v>
+        <v>90800234</v>
       </c>
       <c r="D186" s="2" t="s">
-        <v>33</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E186" s="9"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A187" s="2" t="s">
-        <v>185</v>
+      <c r="A187" s="4" t="s">
+        <v>187</v>
       </c>
       <c r="B187" s="2">
-        <v>90800234</v>
+        <v>1913484</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D187" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E187" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E187" s="7">
+        <v>68510020406</v>
+      </c>
+      <c r="F187" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="4" t="s">
@@ -4420,11 +4422,11 @@
       <c r="D188" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E188" s="11">
-        <v>68510020406</v>
+      <c r="E188">
+        <v>68510020802</v>
       </c>
       <c r="F188" s="2">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -4432,93 +4434,93 @@
         <v>187</v>
       </c>
       <c r="B189" s="2">
-        <v>1913484</v>
+        <v>1913492</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E189" s="11">
-        <v>68510020802</v>
+      <c r="E189">
+        <v>68510021403</v>
       </c>
       <c r="F189" s="2">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B190" s="2">
-        <v>1913492</v>
+        <v>2230584</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E190" s="11">
-        <v>68510021403</v>
+      <c r="E190">
+        <v>68510345400</v>
       </c>
       <c r="F190" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="4" t="s">
+      <c r="A191" s="2" t="s">
         <v>188</v>
       </c>
       <c r="B191" s="2">
-        <v>2230584</v>
+        <v>2230585</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E191">
-        <v>68510345400</v>
-      </c>
-      <c r="F191" s="2">
-        <v>100</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B192" s="2">
-        <v>2230585</v>
+        <v>2238334</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="E192">
+        <v>68510899279</v>
+      </c>
+      <c r="F192" s="2">
+        <v>30</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B193" s="2">
-        <v>2238334</v>
+        <v>593435</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E193">
-        <v>68510899279</v>
+        <v>64589001490</v>
       </c>
       <c r="F193" s="2">
-        <v>30</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -4526,16 +4528,16 @@
         <v>190</v>
       </c>
       <c r="B194" s="2">
-        <v>593435</v>
+        <v>593451</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E194">
-        <v>64589001490</v>
+        <v>64589001575</v>
       </c>
       <c r="F194" s="2">
         <v>100</v>
@@ -4543,42 +4545,42 @@
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="B195" s="2">
-        <v>593451</v>
+        <v>2053403</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="D195" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E195">
-        <v>64589001575</v>
+        <v>64589002916</v>
       </c>
       <c r="F195" s="2">
-        <v>100</v>
+        <v>500</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196" s="2" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B196" s="2">
-        <v>2053403</v>
+        <v>2282941</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="D196" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E196" s="12">
-        <v>64589002916</v>
+        <v>66</v>
+      </c>
+      <c r="E196">
+        <v>68510575128</v>
       </c>
       <c r="F196" s="2">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
@@ -4586,51 +4588,51 @@
         <v>191</v>
       </c>
       <c r="B197" s="2">
-        <v>2282941</v>
+        <v>2282968</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E197">
-        <v>68510575128</v>
-      </c>
-      <c r="F197" s="2">
-        <v>5</v>
-      </c>
+      <c r="E197" s="9"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B198" s="2">
-        <v>2282968</v>
+        <v>653241</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="D198" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E198" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="E198" s="7">
+        <v>64589000752</v>
+      </c>
+      <c r="F198" s="2">
+        <v>500</v>
+      </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B199" s="2">
-        <v>653241</v>
+        <v>653276</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E199">
-        <v>64589000752</v>
+        <v>64589001643</v>
       </c>
       <c r="F199" s="2">
         <v>500</v>
@@ -4638,22 +4640,16 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B200" s="2">
-        <v>653276</v>
+        <v>637742</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>195</v>
+        <v>35</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E200">
-        <v>64589001643</v>
-      </c>
-      <c r="F200" s="2">
-        <v>500</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
@@ -4661,25 +4657,25 @@
         <v>196</v>
       </c>
       <c r="B201" s="2">
-        <v>637742</v>
+        <v>637750</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E201" s="11"/>
+      <c r="E201" s="9"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
         <v>196</v>
       </c>
       <c r="B202" s="2">
-        <v>637750</v>
+        <v>711101</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>8</v>
@@ -4688,34 +4684,39 @@
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B203" s="2">
-        <v>711101</v>
+        <v>2302764</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="D203" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E203" s="7"/>
+      <c r="E203" s="7">
+        <v>68510801333</v>
+      </c>
+      <c r="F203" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="2" t="s">
         <v>197</v>
       </c>
       <c r="B204" s="2">
-        <v>2302764</v>
+        <v>2302772</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D204" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E204">
-        <v>68510801333</v>
+        <v>68510802330</v>
       </c>
       <c r="F204" s="2">
         <v>50</v>
@@ -4726,39 +4727,33 @@
         <v>197</v>
       </c>
       <c r="B205" s="2">
-        <v>2302772</v>
+        <v>2302780</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="D205" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E205" s="11">
-        <v>68510802330</v>
+      <c r="E205">
+        <v>771313162838</v>
       </c>
       <c r="F205" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A206" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B206" s="2">
-        <v>2302780</v>
+        <v>2384884</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E206" s="11">
-        <v>771313162838</v>
-      </c>
-      <c r="F206" s="2">
-        <v>100</v>
+        <v>33</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
@@ -4766,79 +4761,78 @@
         <v>198</v>
       </c>
       <c r="B207" s="2">
-        <v>2384884</v>
+        <v>2384892</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E207" s="11"/>
+      <c r="E207">
+        <v>68510181145</v>
+      </c>
+      <c r="F207" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="2" t="s">
         <v>198</v>
       </c>
       <c r="B208" s="2">
-        <v>2384892</v>
+        <v>2392925</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D208" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E208">
-        <v>68510181145</v>
-      </c>
-      <c r="F208" s="2">
-        <v>50</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B209" s="2">
-        <v>2392925</v>
+        <v>608165</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E209">
+        <v>64589000561</v>
+      </c>
+      <c r="F209" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B210" s="2">
-        <v>608165</v>
+        <v>808571</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="D210" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E210">
-        <v>64589000561</v>
-      </c>
-      <c r="F210" s="2">
-        <v>500</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B211" s="2">
-        <v>808571</v>
+        <v>2163926</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>22</v>
+        <v>195</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>8</v>
@@ -4846,16 +4840,22 @@
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B212" s="2">
-        <v>2163926</v>
+        <v>2322951</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D212" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="E212">
+        <v>354092103102</v>
+      </c>
+      <c r="F212" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -4863,16 +4863,16 @@
         <v>202</v>
       </c>
       <c r="B213" s="2">
-        <v>2322951</v>
+        <v>2322978</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D213" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E213">
-        <v>354092103102</v>
+        <v>354092105106</v>
       </c>
       <c r="F213" s="2">
         <v>100</v>
@@ -4883,16 +4883,16 @@
         <v>202</v>
       </c>
       <c r="B214" s="2">
-        <v>2322978</v>
+        <v>2347156</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D214" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E214">
-        <v>354092105106</v>
+        <v>354092102105</v>
       </c>
       <c r="F214" s="2">
         <v>100</v>
@@ -4903,16 +4903,16 @@
         <v>202</v>
       </c>
       <c r="B215" s="2">
-        <v>2347156</v>
+        <v>2347164</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="D215" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E215">
-        <v>354092102105</v>
+        <v>354092104109</v>
       </c>
       <c r="F215" s="2">
         <v>100</v>
@@ -4923,16 +4923,16 @@
         <v>202</v>
       </c>
       <c r="B216" s="2">
-        <v>2347164</v>
+        <v>2347172</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D216" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E216">
-        <v>354092104109</v>
+      <c r="E216" s="9">
+        <v>354092106103</v>
       </c>
       <c r="F216" s="2">
         <v>100</v>
@@ -4943,16 +4943,16 @@
         <v>202</v>
       </c>
       <c r="B217" s="2">
-        <v>2347172</v>
+        <v>2439603</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="D217" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E217" s="7">
-        <v>354092106103</v>
+        <v>354092101313</v>
       </c>
       <c r="F217" s="2">
         <v>100</v>
@@ -4960,33 +4960,28 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B218" s="2">
-        <v>2439603</v>
+        <v>548359</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E218" s="7">
-        <v>354092101313</v>
-      </c>
-      <c r="F218" s="2">
-        <v>100</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E218" s="7"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="2" t="s">
         <v>203</v>
       </c>
       <c r="B219" s="2">
-        <v>548359</v>
+        <v>548367</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D219" s="2" t="s">
         <v>8</v>
@@ -4994,19 +4989,11 @@
       <c r="E219" s="7"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="B220" s="2">
-        <v>548367</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D220" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E220" s="7"/>
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
+      <c r="C220" s="1"/>
+      <c r="D220" s="1"/>
+      <c r="E220" s="10"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F220">

</xml_diff>

<commit_message>
adding info into the tables
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D82D0-EBED-0646-A88F-D36CFAFF4488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B230D18-0FC6-504F-B3D0-68CA6E97F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="210">
   <si>
     <t>Drug Name</t>
   </si>
@@ -647,6 +647,9 @@
   </si>
   <si>
     <t>SDZ-HYDROMORPHONE IM INJ</t>
+  </si>
+  <si>
+    <t>UNDEF</t>
   </si>
 </sst>
 </file>
@@ -731,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -743,7 +746,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1052,7 +1054,7 @@
   <dimension ref="A1:F220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1098,7 +1100,6 @@
       <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1113,7 +1114,6 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1143,7 +1143,6 @@
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1748,7 +1747,7 @@
       <c r="D40" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40">
         <v>68625100253</v>
       </c>
       <c r="F40" s="2">
@@ -1808,7 +1807,7 @@
       <c r="D43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43">
         <v>886965002392</v>
       </c>
       <c r="F43" s="2">
@@ -1928,7 +1927,6 @@
       <c r="D49" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E49" s="9"/>
       <c r="F49" s="2">
         <v>100</v>
       </c>
@@ -3119,7 +3117,7 @@
       <c r="D116" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E116" s="9">
+      <c r="E116">
         <v>30406000304</v>
       </c>
       <c r="F116" s="2">
@@ -3619,7 +3617,7 @@
       <c r="D144" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E144" s="9">
+      <c r="E144">
         <v>57606022479</v>
       </c>
       <c r="F144" s="2">
@@ -3789,7 +3787,7 @@
       <c r="D153" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E153" s="9">
+      <c r="E153">
         <v>64589000936</v>
       </c>
       <c r="F153" s="2">
@@ -4167,7 +4165,7 @@
       <c r="D174" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E174" s="9">
+      <c r="E174">
         <v>628791004764</v>
       </c>
       <c r="F174" s="2">
@@ -4261,7 +4259,6 @@
       <c r="D179" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E179" s="9"/>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
@@ -4384,10 +4381,12 @@
       <c r="B186" s="2">
         <v>90800234</v>
       </c>
+      <c r="C186" s="2" t="s">
+        <v>209</v>
+      </c>
       <c r="D186" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E186" s="9"/>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="4" t="s">
@@ -4596,7 +4595,6 @@
       <c r="D197" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E197" s="9"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="2" t="s">
@@ -4665,7 +4663,6 @@
       <c r="D201" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E201" s="9"/>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A202" s="2" t="s">
@@ -4931,7 +4928,7 @@
       <c r="D216" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E216" s="9">
+      <c r="E216">
         <v>354092106103</v>
       </c>
       <c r="F216" s="2">
@@ -4993,7 +4990,7 @@
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
-      <c r="E220" s="10"/>
+      <c r="E220" s="9"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F220">

</xml_diff>

<commit_message>
find narcs by upc function is working with the new tables with the din as primary key
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B230D18-0FC6-504F-B3D0-68CA6E97F86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9332554-8429-B647-91A8-85FFB359A466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="209">
   <si>
     <t>Drug Name</t>
   </si>
@@ -647,9 +647,6 @@
   </si>
   <si>
     <t>SDZ-HYDROMORPHONE IM INJ</t>
-  </si>
-  <si>
-    <t>UNDEF</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C180" sqref="C180"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E182" sqref="E182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4382,7 +4379,7 @@
         <v>90800234</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>209</v>
+        <v>87</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
Added a new step in README
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9332554-8429-B647-91A8-85FFB359A466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D1F82-ACC7-CC4D-8509-FCECCB75DCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E182" sqref="E182"/>
+    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Function to add is working and refreshes the page after each click
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095D1F82-ACC7-CC4D-8509-FCECCB75DCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3530D43-4C17-5C4D-A703-2961AD467DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B177" sqref="B177"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Made the set_quantity function for reconsiliation, next i will do the audit_log
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradley-hansdesmornes/Documents/projects/Narc_Recon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3530D43-4C17-5C4D-A703-2961AD467DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5880B22C-7935-1B46-9D6F-4F331077009C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1050,8 +1050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F222" sqref="A220:F222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4983,8 +4983,6 @@
       <c r="E219" s="7"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" s="1"/>
-      <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
       <c r="E220" s="9"/>

</xml_diff>

<commit_message>
updated everything with other version i was working on for the pharmacy
</commit_message>
<xml_diff>
--- a/Sheet1.xlsx
+++ b/Sheet1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Documents/projects/Narc_Recon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5880B22C-7935-1B46-9D6F-4F331077009C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD725DB-92C8-054F-B8B5-7CC8489EA1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="740" windowWidth="25600" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="215">
   <si>
     <t>Drug Name</t>
   </si>
@@ -647,6 +647,24 @@
   </si>
   <si>
     <t>SDZ-HYDROMORPHONE IM INJ</t>
+  </si>
+  <si>
+    <t>0.5mg</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>egdd</t>
+  </si>
+  <si>
+    <t>sfgw</t>
+  </si>
+  <si>
+    <t>egddafsoaso</t>
   </si>
 </sst>
 </file>
@@ -731,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -744,6 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F220"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F222" sqref="A220:F222"/>
+    <sheetView tabSelected="1" topLeftCell="A202" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E226" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3990,7 +4009,7 @@
         <v>165</v>
       </c>
       <c r="B164" s="2">
-        <v>2457344</v>
+        <v>2457334</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>114</v>
@@ -4983,9 +5002,104 @@
       <c r="E219" s="7"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C220" s="1"/>
-      <c r="D220" s="1"/>
-      <c r="E220" s="9"/>
+      <c r="A220" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B220" s="2">
+        <v>13343</v>
+      </c>
+      <c r="C220" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E220" s="9">
+        <v>32948709</v>
+      </c>
+      <c r="F220" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B221" s="2">
+        <v>164345</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D221" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E221" s="9">
+        <v>4645</v>
+      </c>
+      <c r="F221" s="2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B222" s="2">
+        <v>123534</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E222" s="9">
+        <v>54646</v>
+      </c>
+      <c r="F222" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B223" s="2">
+        <v>45664</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D223" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E223" s="10">
+        <v>3456764</v>
+      </c>
+      <c r="F223" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B224" s="2">
+        <v>46543</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E224" s="9">
+        <v>859373</v>
+      </c>
+      <c r="F224" s="2">
+        <v>150</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F220">

</xml_diff>